<commit_message>
set default old script and template
</commit_message>
<xml_diff>
--- a/global_variable_template.xlsx
+++ b/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15120" windowHeight="14220" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15120" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -1599,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2369,7 +2369,7 @@
   <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2928,7 +2928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>

</xml_diff>